<commit_message>
corrected s1cDNA file names to confrom to stanadard
</commit_message>
<xml_diff>
--- a/fastqFiles/fastqFiles_09.27.19.xlsx
+++ b/fastqFiles/fastqFiles_09.27.19.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4322B7-642F-D440-B35A-4A9F48A32173}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9854996-9E14-B946-A09B-6218FB35E66F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24060" windowHeight="17880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="71">
   <si>
     <t>libraryDate</t>
   </si>
@@ -217,13 +217,34 @@
   </si>
   <si>
     <t>08.09.19</t>
+  </si>
+  <si>
+    <t>Brent_2c-20_GTAC_60_SIC_Index2_6_CTGCAAT_GACCTTGT_S21_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2c-21_GTAC_61_SIC_Index2_6_CAAGCCG_GACCTTGT_S22_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2c-22_GTAC_62_SIC_Index2_6_GGGTCAA_GACCTTGT_S23_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2c-23_GTAC_63_SIC_Index2_6_GCAACGC_GACCTTGT_S24_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2c-24_GTAC_64_SIC_Index2_6_TGATTAC_GACCTTGT_S25_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2c-25_GTAC_65_SIC_Index2_6_TGCTGGG_GACCTTGT_S26_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_2c-26_GTAC_66_SIC_Index2_6_GACACAG_GACCTTGT_S27_R1_001.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -258,6 +279,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -279,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -297,6 +324,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y46"/>
+  <dimension ref="A1:Y53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A20"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1352,284 +1381,284 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3906</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21" s="9">
+        <v>437</v>
+      </c>
+      <c r="K21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22" s="5">
+        <v>3906</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22" s="10">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3906</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23" s="9">
+        <v>2</v>
+      </c>
+      <c r="K23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24" s="5">
+        <v>3906</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24" s="10">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25" s="5">
+        <v>3906</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25" s="9">
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26" s="5">
+        <v>3906</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26" s="9">
+        <v>2</v>
+      </c>
+      <c r="K26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3906</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27" s="9">
+        <v>9</v>
+      </c>
+      <c r="K27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="4">
         <v>1</v>
       </c>
-      <c r="D21">
-        <v>3906</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="D28">
+        <v>3906</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="8">
+      <c r="G28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="8">
         <v>156</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I28" s="8">
         <v>0.87324960960960996</v>
       </c>
-      <c r="J21">
+      <c r="J28">
         <v>6628739</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K28" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>3906</v>
-      </c>
-      <c r="E22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22">
-        <v>205</v>
-      </c>
-      <c r="I22">
-        <v>0.76053908722374797</v>
-      </c>
-      <c r="J22">
-        <v>7246147</v>
-      </c>
-      <c r="K22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>3906</v>
-      </c>
-      <c r="E23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23">
-        <v>99.5</v>
-      </c>
-      <c r="I23">
-        <v>1.0090817038258</v>
-      </c>
-      <c r="J23">
-        <v>7033022</v>
-      </c>
-      <c r="K23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>3906</v>
-      </c>
-      <c r="E24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24">
-        <v>153</v>
-      </c>
-      <c r="I24">
-        <v>1.1201545454545501</v>
-      </c>
-      <c r="J24">
-        <v>5830709</v>
-      </c>
-      <c r="K24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25">
-        <v>5</v>
-      </c>
-      <c r="D25">
-        <v>3906</v>
-      </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25">
-        <v>24.9</v>
-      </c>
-      <c r="I25">
-        <v>0.56412458412144095</v>
-      </c>
-      <c r="J25">
-        <v>6602748</v>
-      </c>
-      <c r="K25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26">
-        <v>6</v>
-      </c>
-      <c r="D26">
-        <v>3906</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26">
-        <v>47.1</v>
-      </c>
-      <c r="I26">
-        <v>0.90301100846207605</v>
-      </c>
-      <c r="J26">
-        <v>5364357</v>
-      </c>
-      <c r="K26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27">
-        <v>7</v>
-      </c>
-      <c r="D27">
-        <v>3906</v>
-      </c>
-      <c r="E27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27">
-        <v>5.72</v>
-      </c>
-      <c r="I27">
-        <v>1.5565167657938099</v>
-      </c>
-      <c r="J27">
-        <v>8176651</v>
-      </c>
-      <c r="K27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28">
-        <v>8</v>
-      </c>
-      <c r="D28">
-        <v>3906</v>
-      </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28">
-        <v>20.9</v>
-      </c>
-      <c r="I28">
-        <v>0.66275518076408102</v>
-      </c>
-      <c r="J28">
-        <v>7535848</v>
-      </c>
-      <c r="K28" t="s">
-        <v>43</v>
-      </c>
+      <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1639,7 +1668,7 @@
         <v>11</v>
       </c>
       <c r="C29">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D29">
         <v>3906</v>
@@ -1654,16 +1683,16 @@
         <v>14</v>
       </c>
       <c r="H29">
-        <v>272</v>
+        <v>205</v>
       </c>
       <c r="I29">
-        <v>0.86933369207772804</v>
+        <v>0.76053908722374797</v>
       </c>
       <c r="J29">
-        <v>7591733</v>
+        <v>7246147</v>
       </c>
       <c r="K29" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -1674,7 +1703,7 @@
         <v>11</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D30">
         <v>3906</v>
@@ -1689,16 +1718,16 @@
         <v>14</v>
       </c>
       <c r="H30">
-        <v>181</v>
+        <v>99.5</v>
       </c>
       <c r="I30">
-        <v>1.0020403859407301</v>
+        <v>1.0090817038258</v>
       </c>
       <c r="J30">
-        <v>6284042</v>
+        <v>7033022</v>
       </c>
       <c r="K30" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -1709,7 +1738,7 @@
         <v>11</v>
       </c>
       <c r="C31">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D31">
         <v>3906</v>
@@ -1724,16 +1753,16 @@
         <v>14</v>
       </c>
       <c r="H31">
-        <v>211</v>
+        <v>153</v>
       </c>
       <c r="I31">
-        <v>0.80257260746567305</v>
+        <v>1.1201545454545501</v>
       </c>
       <c r="J31">
-        <v>7185205</v>
+        <v>5830709</v>
       </c>
       <c r="K31" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -1744,7 +1773,7 @@
         <v>11</v>
       </c>
       <c r="C32">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D32">
         <v>3906</v>
@@ -1759,16 +1788,16 @@
         <v>14</v>
       </c>
       <c r="H32">
-        <v>225</v>
+        <v>24.9</v>
       </c>
       <c r="I32">
-        <v>0.96472462469934495</v>
+        <v>0.56412458412144095</v>
       </c>
       <c r="J32">
-        <v>5686830</v>
+        <v>6602748</v>
       </c>
       <c r="K32" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1779,7 +1808,7 @@
         <v>11</v>
       </c>
       <c r="C33">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D33">
         <v>3906</v>
@@ -1794,16 +1823,16 @@
         <v>14</v>
       </c>
       <c r="H33">
-        <v>205</v>
+        <v>47.1</v>
       </c>
       <c r="I33">
-        <v>0.65641562076749405</v>
+        <v>0.90301100846207605</v>
       </c>
       <c r="J33">
-        <v>6371816</v>
+        <v>5364357</v>
       </c>
       <c r="K33" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -1814,7 +1843,7 @@
         <v>11</v>
       </c>
       <c r="C34">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D34">
         <v>3906</v>
@@ -1829,16 +1858,16 @@
         <v>14</v>
       </c>
       <c r="H34">
-        <v>67</v>
+        <v>5.72</v>
       </c>
       <c r="I34">
-        <v>0.84357869238858496</v>
+        <v>1.5565167657938099</v>
       </c>
       <c r="J34">
-        <v>5108335</v>
+        <v>8176651</v>
       </c>
       <c r="K34" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1849,7 +1878,7 @@
         <v>11</v>
       </c>
       <c r="C35">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D35">
         <v>3906</v>
@@ -1864,16 +1893,16 @@
         <v>14</v>
       </c>
       <c r="H35">
-        <v>188</v>
+        <v>20.9</v>
       </c>
       <c r="I35">
-        <v>0.94149377150026303</v>
+        <v>0.66275518076408102</v>
       </c>
       <c r="J35">
-        <v>6319000</v>
+        <v>7535848</v>
       </c>
       <c r="K35" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
@@ -1884,7 +1913,7 @@
         <v>11</v>
       </c>
       <c r="C36">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D36">
         <v>3906</v>
@@ -1899,16 +1928,16 @@
         <v>14</v>
       </c>
       <c r="H36">
-        <v>118</v>
+        <v>272</v>
       </c>
       <c r="I36">
-        <v>0.59074072117826304</v>
+        <v>0.86933369207772804</v>
       </c>
       <c r="J36">
-        <v>7659797</v>
+        <v>7591733</v>
       </c>
       <c r="K36" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -1919,7 +1948,7 @@
         <v>11</v>
       </c>
       <c r="C37">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D37">
         <v>3906</v>
@@ -1934,10 +1963,16 @@
         <v>14</v>
       </c>
       <c r="H37">
-        <v>0.28299999999999997</v>
+        <v>181</v>
+      </c>
+      <c r="I37">
+        <v>1.0020403859407301</v>
+      </c>
+      <c r="J37">
+        <v>6284042</v>
       </c>
       <c r="K37" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1948,7 +1983,7 @@
         <v>11</v>
       </c>
       <c r="C38">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D38">
         <v>3906</v>
@@ -1963,16 +1998,16 @@
         <v>14</v>
       </c>
       <c r="H38">
-        <v>16.399999999999999</v>
+        <v>211</v>
       </c>
       <c r="I38">
-        <v>1.46411791805652</v>
+        <v>0.80257260746567305</v>
       </c>
       <c r="J38">
-        <v>9800442</v>
+        <v>7185205</v>
       </c>
       <c r="K38" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -1983,7 +2018,7 @@
         <v>11</v>
       </c>
       <c r="C39">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D39">
         <v>3906</v>
@@ -1998,16 +2033,16 @@
         <v>14</v>
       </c>
       <c r="H39">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="I39">
-        <v>0.81677443999719102</v>
+        <v>0.96472462469934495</v>
       </c>
       <c r="J39">
-        <v>6717693</v>
+        <v>5686830</v>
       </c>
       <c r="K39" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2018,7 +2053,7 @@
         <v>11</v>
       </c>
       <c r="C40">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D40">
         <v>3906</v>
@@ -2033,16 +2068,16 @@
         <v>14</v>
       </c>
       <c r="H40">
-        <v>253</v>
+        <v>205</v>
       </c>
       <c r="I40">
-        <v>0.84004512331636205</v>
+        <v>0.65641562076749405</v>
       </c>
       <c r="J40">
-        <v>6649107</v>
+        <v>6371816</v>
       </c>
       <c r="K40" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2053,7 +2088,7 @@
         <v>11</v>
       </c>
       <c r="C41">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D41">
         <v>3906</v>
@@ -2068,10 +2103,16 @@
         <v>14</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="I41">
+        <v>0.84357869238858496</v>
+      </c>
+      <c r="J41">
+        <v>5108335</v>
       </c>
       <c r="K41" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2082,7 +2123,7 @@
         <v>11</v>
       </c>
       <c r="C42">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D42">
         <v>3906</v>
@@ -2097,13 +2138,16 @@
         <v>14</v>
       </c>
       <c r="H42">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="I42" t="s">
-        <v>57</v>
+        <v>188</v>
+      </c>
+      <c r="I42">
+        <v>0.94149377150026303</v>
+      </c>
+      <c r="J42">
+        <v>6319000</v>
       </c>
       <c r="K42" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -2114,7 +2158,7 @@
         <v>11</v>
       </c>
       <c r="C43">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D43">
         <v>3906</v>
@@ -2129,10 +2173,16 @@
         <v>14</v>
       </c>
       <c r="H43">
-        <v>0.42199999999999999</v>
+        <v>118</v>
+      </c>
+      <c r="I43">
+        <v>0.59074072117826304</v>
+      </c>
+      <c r="J43">
+        <v>7659797</v>
       </c>
       <c r="K43" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2143,7 +2193,7 @@
         <v>11</v>
       </c>
       <c r="C44">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D44">
         <v>3906</v>
@@ -2158,10 +2208,10 @@
         <v>14</v>
       </c>
       <c r="H44">
-        <v>0.317</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="K44" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -2172,7 +2222,7 @@
         <v>11</v>
       </c>
       <c r="C45">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D45">
         <v>3906</v>
@@ -2187,16 +2237,16 @@
         <v>14</v>
       </c>
       <c r="H45">
-        <v>233</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="I45">
-        <v>0.84272304292700595</v>
+        <v>1.46411791805652</v>
       </c>
       <c r="J45">
-        <v>6395198</v>
+        <v>9800442</v>
       </c>
       <c r="K45" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -2207,7 +2257,7 @@
         <v>11</v>
       </c>
       <c r="C46">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D46">
         <v>3906</v>
@@ -2222,15 +2272,239 @@
         <v>14</v>
       </c>
       <c r="H46">
+        <v>233</v>
+      </c>
+      <c r="I46">
+        <v>0.81677443999719102</v>
+      </c>
+      <c r="J46">
+        <v>6717693</v>
+      </c>
+      <c r="K46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+      <c r="D47">
+        <v>3906</v>
+      </c>
+      <c r="E47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G47" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47">
+        <v>253</v>
+      </c>
+      <c r="I47">
+        <v>0.84004512331636205</v>
+      </c>
+      <c r="J47">
+        <v>6649107</v>
+      </c>
+      <c r="K47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>21</v>
+      </c>
+      <c r="D48">
+        <v>3906</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" t="s">
+        <v>35</v>
+      </c>
+      <c r="G48" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="K48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <v>22</v>
+      </c>
+      <c r="D49">
+        <v>3906</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" t="s">
+        <v>35</v>
+      </c>
+      <c r="G49" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="I49" t="s">
+        <v>57</v>
+      </c>
+      <c r="K49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50">
+        <v>23</v>
+      </c>
+      <c r="D50">
+        <v>3906</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="K50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51">
+        <v>24</v>
+      </c>
+      <c r="D51">
+        <v>3906</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51">
+        <v>0.317</v>
+      </c>
+      <c r="K51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52">
+        <v>25</v>
+      </c>
+      <c r="D52">
+        <v>3906</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52">
+        <v>233</v>
+      </c>
+      <c r="I52">
+        <v>0.84272304292700595</v>
+      </c>
+      <c r="J52">
+        <v>6395198</v>
+      </c>
+      <c r="K52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>26</v>
+      </c>
+      <c r="D53">
+        <v>3906</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53">
         <v>181</v>
       </c>
-      <c r="I46">
+      <c r="I53">
         <v>1.06065607076095</v>
       </c>
-      <c r="J46">
+      <c r="J53">
         <v>6850105</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K53" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>